<commit_message>
Bazı formlarda resim gözükmeme sorunu çözüldü.
</commit_message>
<xml_diff>
--- a/backend/form_sablonlari/F.02 Üretim İş Emri Formu.xlsx
+++ b/backend/form_sablonlari/F.02 Üretim İş Emri Formu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duran Ozcelik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC785844-7820-49D9-8D00-CE9631409D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B3D597-E913-48F0-9A61-09D03B937CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="152">
   <si>
     <t>PARÇA NUMARASI</t>
   </si>
@@ -1759,6 +1759,15 @@
     <xf numFmtId="49" fontId="11" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1860,15 +1869,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2102,18 +2102,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2128,6 +2125,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2567,13 +2567,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3202,22 +3202,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2598</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1029083</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:rowOff>163789</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Resim 2">
+        <xdr:cNvPr id="2" name="Resim 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14C35833-9367-4EAF-9CA8-28EEB848662B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD8902FA-39E1-1159-AFD4-70C7E2E84827}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3233,8 +3233,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="247650" y="57150"/>
-          <a:ext cx="2800350" cy="952500"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2743583" cy="943107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>294409</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>186364</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63402</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Resim 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F034A7A6-B984-9635-68EA-408928E1046F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9213273" y="3861955"/>
+          <a:ext cx="1381318" cy="1362265"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4198,7 +4242,7 @@
   <dimension ref="A1:T55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="L10" sqref="L10:Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4320,13 +4364,13 @@
       </c>
       <c r="B5" s="166"/>
       <c r="C5" s="167"/>
-      <c r="D5" s="176"/>
+      <c r="D5" s="175"/>
       <c r="E5" s="153"/>
       <c r="F5" s="154"/>
-      <c r="G5" s="172" t="s">
+      <c r="G5" s="171" t="s">
         <v>149</v>
       </c>
-      <c r="H5" s="173"/>
+      <c r="H5" s="172"/>
       <c r="I5" s="152"/>
       <c r="J5" s="153"/>
       <c r="K5" s="154"/>
@@ -4345,16 +4389,16 @@
       </c>
       <c r="B6" s="96"/>
       <c r="C6" s="97"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="91"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="170"/>
       <c r="G6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H6" s="8"/>
-      <c r="I6" s="321"/>
-      <c r="J6" s="322"/>
-      <c r="K6" s="323"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
       <c r="L6" s="95" t="s">
         <v>5</v>
       </c>
@@ -4373,13 +4417,13 @@
       <c r="D7" s="92"/>
       <c r="E7" s="93"/>
       <c r="F7" s="94"/>
-      <c r="G7" s="174" t="s">
+      <c r="G7" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="175"/>
-      <c r="I7" s="171"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="91"/>
+      <c r="H7" s="174"/>
+      <c r="I7" s="168"/>
+      <c r="J7" s="169"/>
+      <c r="K7" s="170"/>
       <c r="L7" s="95" t="s">
         <v>97</v>
       </c>
@@ -4415,18 +4459,18 @@
       <c r="Q8" s="157"/>
     </row>
     <row r="9" spans="1:17" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="112"/>
       <c r="E9" s="113"/>
       <c r="F9" s="114"/>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="62"/>
+      <c r="H9" s="65"/>
       <c r="I9" s="129"/>
       <c r="J9" s="130"/>
       <c r="K9" s="131"/>
@@ -4440,11 +4484,11 @@
       <c r="Q9" s="100"/>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="115" t="s">
         <v>40</v>
       </c>
@@ -4457,9 +4501,7 @@
       <c r="I10" s="118"/>
       <c r="J10" s="118"/>
       <c r="K10" s="119"/>
-      <c r="L10" s="120" t="s">
-        <v>24</v>
-      </c>
+      <c r="L10" s="120"/>
       <c r="M10" s="121"/>
       <c r="N10" s="121"/>
       <c r="O10" s="121"/>
@@ -4467,23 +4509,23 @@
       <c r="Q10" s="122"/>
     </row>
     <row r="11" spans="1:17" s="3" customFormat="1" ht="124.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="65" t="s">
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="65" t="s">
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="123" t="s">
         <v>55</v>
       </c>
@@ -4494,21 +4536,21 @@
       <c r="Q11" s="125"/>
     </row>
     <row r="12" spans="1:17" s="3" customFormat="1" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="69" t="s">
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="73"/>
       <c r="L12" s="126"/>
       <c r="M12" s="127"/>
       <c r="N12" s="127"/>
@@ -4517,34 +4559,34 @@
       <c r="Q12" s="128"/>
     </row>
     <row r="13" spans="1:17" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="60"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="63"/>
     </row>
     <row r="14" spans="1:17" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="64"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="106" t="s">
         <v>98</v>
       </c>
@@ -4580,184 +4622,184 @@
       <c r="A15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="81"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="84"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="85"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="88"/>
       <c r="K15" s="12"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
-      <c r="N15" s="86"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="88"/>
+      <c r="N15" s="89"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="91"/>
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="1:17" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="81"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="85"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="88"/>
       <c r="K16" s="12"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="86"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="88"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="90"/>
+      <c r="P16" s="91"/>
       <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="1:17" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="84"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="85"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="88"/>
       <c r="K17" s="12"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
-      <c r="N17" s="86"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="88"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="91"/>
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="1:17" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="83"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="81"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="84"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="85"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="88"/>
       <c r="K18" s="12"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
-      <c r="N18" s="86"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="88"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="91"/>
       <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="1:17" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="83"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="81"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="84"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="85"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="88"/>
       <c r="K19" s="12"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
-      <c r="N19" s="86"/>
-      <c r="O19" s="87"/>
-      <c r="P19" s="88"/>
+      <c r="N19" s="89"/>
+      <c r="O19" s="90"/>
+      <c r="P19" s="91"/>
       <c r="Q19" s="10"/>
     </row>
     <row r="20" spans="1:17" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="83"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="81"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="84"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="84"/>
-      <c r="J20" s="85"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="88"/>
       <c r="K20" s="12"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
-      <c r="N20" s="86"/>
-      <c r="O20" s="87"/>
-      <c r="P20" s="88"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="90"/>
+      <c r="P20" s="91"/>
       <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="1:17" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="81"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="85"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="88"/>
       <c r="K21" s="12"/>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
-      <c r="N21" s="86"/>
-      <c r="O21" s="87"/>
-      <c r="P21" s="88"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="90"/>
+      <c r="P21" s="91"/>
       <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="1:17" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="83"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="81"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="84"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="85"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="88"/>
       <c r="K22" s="12"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
-      <c r="N22" s="86"/>
-      <c r="O22" s="87"/>
-      <c r="P22" s="88"/>
+      <c r="N22" s="89"/>
+      <c r="O22" s="90"/>
+      <c r="P22" s="91"/>
       <c r="Q22" s="10"/>
     </row>
     <row r="23" spans="1:17" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4978,30 +5020,30 @@
       <c r="Q31" s="21"/>
     </row>
     <row r="32" spans="1:17" ht="195.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="71" t="s">
+      <c r="B32" s="78"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="65" t="s">
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="76"/>
+      <c r="L32" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="M32" s="67"/>
-      <c r="N32" s="77" t="s">
+      <c r="M32" s="70"/>
+      <c r="N32" s="80" t="s">
         <v>151</v>
       </c>
-      <c r="O32" s="78"/>
-      <c r="P32" s="78"/>
+      <c r="O32" s="81"/>
+      <c r="P32" s="81"/>
       <c r="Q32" s="16" t="s">
         <v>102</v>
       </c>
@@ -5535,17 +5577,17 @@
       </c>
       <c r="B5" s="166"/>
       <c r="C5" s="167"/>
-      <c r="D5" s="176">
+      <c r="D5" s="175">
         <f>ANA!D5</f>
         <v>0</v>
       </c>
       <c r="E5" s="153"/>
       <c r="F5" s="154"/>
-      <c r="G5" s="172" t="s">
+      <c r="G5" s="171" t="s">
         <v>149</v>
       </c>
-      <c r="H5" s="173"/>
-      <c r="I5" s="176">
+      <c r="H5" s="172"/>
+      <c r="I5" s="175">
         <f>ANA!I5</f>
         <v>0</v>
       </c>
@@ -5556,7 +5598,7 @@
       </c>
       <c r="M5" s="163"/>
       <c r="N5" s="164"/>
-      <c r="O5" s="176">
+      <c r="O5" s="175">
         <f>ANA!O5</f>
         <v>0</v>
       </c>
@@ -5609,10 +5651,10 @@
       </c>
       <c r="E7" s="222"/>
       <c r="F7" s="223"/>
-      <c r="G7" s="174" t="s">
+      <c r="G7" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="175"/>
+      <c r="H7" s="174"/>
       <c r="I7" s="221">
         <f>ANA!I7</f>
         <v>0</v>
@@ -5666,21 +5708,21 @@
       <c r="Q8" s="223"/>
     </row>
     <row r="9" spans="1:17" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="237">
         <f>ANA!D9</f>
         <v>0</v>
       </c>
       <c r="E9" s="238"/>
       <c r="F9" s="239"/>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="62"/>
+      <c r="H9" s="65"/>
       <c r="I9" s="237">
         <f>ANA!I9</f>
         <v>0</v>
@@ -6089,11 +6131,11 @@
       <c r="A22" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="66" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="268"/>
-      <c r="D22" s="64"/>
+      <c r="D22" s="67"/>
       <c r="E22" s="106" t="s">
         <v>32</v>
       </c>
@@ -6653,17 +6695,17 @@
       </c>
       <c r="B5" s="166"/>
       <c r="C5" s="167"/>
-      <c r="D5" s="176">
+      <c r="D5" s="175">
         <f>ANA!D5</f>
         <v>0</v>
       </c>
       <c r="E5" s="153"/>
       <c r="F5" s="154"/>
-      <c r="G5" s="172" t="s">
+      <c r="G5" s="171" t="s">
         <v>149</v>
       </c>
-      <c r="H5" s="173"/>
-      <c r="I5" s="176">
+      <c r="H5" s="172"/>
+      <c r="I5" s="175">
         <f>ANA!I5</f>
         <v>0</v>
       </c>
@@ -6674,7 +6716,7 @@
       </c>
       <c r="M5" s="163"/>
       <c r="N5" s="164"/>
-      <c r="O5" s="176">
+      <c r="O5" s="175">
         <f>ANA!O5</f>
         <v>0</v>
       </c>
@@ -6727,10 +6769,10 @@
       </c>
       <c r="E7" s="222"/>
       <c r="F7" s="223"/>
-      <c r="G7" s="174" t="s">
+      <c r="G7" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="175"/>
+      <c r="H7" s="174"/>
       <c r="I7" s="221">
         <f>ANA!I7</f>
         <v>0</v>
@@ -6784,21 +6826,21 @@
       <c r="Q8" s="223"/>
     </row>
     <row r="9" spans="1:17" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="237">
         <f>ANA!D9</f>
         <v>0</v>
       </c>
       <c r="E9" s="238"/>
       <c r="F9" s="239"/>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="62"/>
+      <c r="H9" s="65"/>
       <c r="I9" s="237">
         <f>ANA!I9</f>
         <v>0</v>
@@ -6881,21 +6923,21 @@
       <c r="A12" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="83"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="81"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="84"/>
       <c r="H12" s="48"/>
       <c r="I12" s="49"/>
       <c r="J12" s="50"/>
-      <c r="K12" s="82" t="s">
+      <c r="K12" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L12" s="83"/>
+      <c r="L12" s="86"/>
       <c r="M12" s="52"/>
       <c r="N12" s="316"/>
       <c r="O12" s="317"/>
@@ -6906,21 +6948,21 @@
       <c r="A13" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="81"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="84"/>
       <c r="H13" s="48"/>
       <c r="I13" s="49"/>
       <c r="J13" s="50"/>
-      <c r="K13" s="82" t="s">
+      <c r="K13" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L13" s="83"/>
+      <c r="L13" s="86"/>
       <c r="M13" s="52"/>
       <c r="N13" s="316"/>
       <c r="O13" s="317"/>
@@ -6931,21 +6973,21 @@
       <c r="A14" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="83"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="81"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="84"/>
       <c r="H14" s="48"/>
       <c r="I14" s="49"/>
       <c r="J14" s="50"/>
-      <c r="K14" s="82" t="s">
+      <c r="K14" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L14" s="83"/>
+      <c r="L14" s="86"/>
       <c r="M14" s="52"/>
       <c r="N14" s="316"/>
       <c r="O14" s="317"/>
@@ -6956,21 +6998,21 @@
       <c r="A15" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="81"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="84"/>
       <c r="H15" s="48"/>
       <c r="I15" s="49"/>
       <c r="J15" s="50"/>
-      <c r="K15" s="82" t="s">
+      <c r="K15" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L15" s="83"/>
+      <c r="L15" s="86"/>
       <c r="M15" s="52"/>
       <c r="N15" s="316"/>
       <c r="O15" s="317"/>
@@ -6981,21 +7023,21 @@
       <c r="A16" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="81"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="48"/>
       <c r="I16" s="49"/>
       <c r="J16" s="50"/>
-      <c r="K16" s="82" t="s">
+      <c r="K16" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L16" s="83"/>
+      <c r="L16" s="86"/>
       <c r="M16" s="52"/>
       <c r="N16" s="316"/>
       <c r="O16" s="317"/>
@@ -7006,21 +7048,21 @@
       <c r="A17" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="84"/>
       <c r="H17" s="48"/>
       <c r="I17" s="49"/>
       <c r="J17" s="50"/>
-      <c r="K17" s="82" t="s">
+      <c r="K17" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L17" s="83"/>
+      <c r="L17" s="86"/>
       <c r="M17" s="52"/>
       <c r="N17" s="316"/>
       <c r="O17" s="317"/>
@@ -7031,21 +7073,21 @@
       <c r="A18" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="83"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="81"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="84"/>
       <c r="H18" s="48"/>
       <c r="I18" s="49"/>
       <c r="J18" s="50"/>
-      <c r="K18" s="82" t="s">
+      <c r="K18" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L18" s="83"/>
+      <c r="L18" s="86"/>
       <c r="M18" s="52"/>
       <c r="N18" s="316"/>
       <c r="O18" s="317"/>
@@ -7056,21 +7098,21 @@
       <c r="A19" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="83"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="81"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="84"/>
       <c r="H19" s="48"/>
       <c r="I19" s="49"/>
       <c r="J19" s="50"/>
-      <c r="K19" s="82" t="s">
+      <c r="K19" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L19" s="83"/>
+      <c r="L19" s="86"/>
       <c r="M19" s="52"/>
       <c r="N19" s="316"/>
       <c r="O19" s="317"/>
@@ -7083,21 +7125,21 @@
       <c r="A20" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C20" s="83"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="81"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="84"/>
       <c r="H20" s="48"/>
       <c r="I20" s="49"/>
       <c r="J20" s="50"/>
-      <c r="K20" s="82" t="s">
+      <c r="K20" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L20" s="83"/>
+      <c r="L20" s="86"/>
       <c r="M20" s="52"/>
       <c r="N20" s="316"/>
       <c r="O20" s="317"/>
@@ -7110,21 +7152,21 @@
       <c r="A21" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="81"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="48"/>
       <c r="I21" s="49"/>
       <c r="J21" s="50"/>
-      <c r="K21" s="82" t="s">
+      <c r="K21" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L21" s="83"/>
+      <c r="L21" s="86"/>
       <c r="M21" s="52"/>
       <c r="N21" s="316"/>
       <c r="O21" s="317"/>
@@ -7137,21 +7179,21 @@
       <c r="A22" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="83"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="81"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="84"/>
       <c r="H22" s="48"/>
       <c r="I22" s="49"/>
       <c r="J22" s="50"/>
-      <c r="K22" s="82" t="s">
+      <c r="K22" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L22" s="83"/>
+      <c r="L22" s="86"/>
       <c r="M22" s="52"/>
       <c r="N22" s="316"/>
       <c r="O22" s="317"/>
@@ -7164,21 +7206,21 @@
       <c r="A23" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="79"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="81"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="84"/>
       <c r="H23" s="48"/>
       <c r="I23" s="49"/>
       <c r="J23" s="50"/>
-      <c r="K23" s="82" t="s">
+      <c r="K23" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="L23" s="83"/>
+      <c r="L23" s="86"/>
       <c r="M23" s="52"/>
       <c r="N23" s="316"/>
       <c r="O23" s="317"/>
@@ -7438,13 +7480,13 @@
       </c>
       <c r="B5" s="166"/>
       <c r="C5" s="167"/>
-      <c r="D5" s="176"/>
+      <c r="D5" s="175"/>
       <c r="E5" s="153"/>
       <c r="F5" s="154"/>
-      <c r="G5" s="172" t="s">
+      <c r="G5" s="171" t="s">
         <v>149</v>
       </c>
-      <c r="H5" s="173"/>
+      <c r="H5" s="172"/>
       <c r="I5" s="152"/>
       <c r="J5" s="153"/>
       <c r="K5" s="154"/>
@@ -7463,16 +7505,16 @@
       </c>
       <c r="B6" s="96"/>
       <c r="C6" s="97"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="91"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="170"/>
       <c r="G6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H6" s="8"/>
-      <c r="I6" s="168"/>
-      <c r="J6" s="169"/>
-      <c r="K6" s="170"/>
+      <c r="I6" s="321"/>
+      <c r="J6" s="322"/>
+      <c r="K6" s="323"/>
       <c r="L6" s="95" t="s">
         <v>5</v>
       </c>
@@ -7491,13 +7533,13 @@
       <c r="D7" s="92"/>
       <c r="E7" s="93"/>
       <c r="F7" s="94"/>
-      <c r="G7" s="174" t="s">
+      <c r="G7" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="175"/>
-      <c r="I7" s="171"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="91"/>
+      <c r="H7" s="174"/>
+      <c r="I7" s="168"/>
+      <c r="J7" s="169"/>
+      <c r="K7" s="170"/>
       <c r="L7" s="95" t="s">
         <v>97</v>
       </c>
@@ -7533,18 +7575,18 @@
       <c r="Q8" s="157"/>
     </row>
     <row r="9" spans="1:17" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="112"/>
       <c r="E9" s="113"/>
       <c r="F9" s="114"/>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="62"/>
+      <c r="H9" s="65"/>
       <c r="I9" s="129"/>
       <c r="J9" s="130"/>
       <c r="K9" s="131"/>
@@ -7558,11 +7600,11 @@
       <c r="Q9" s="100"/>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="115" t="s">
         <v>40</v>
       </c>
@@ -7585,23 +7627,23 @@
       <c r="Q10" s="122"/>
     </row>
     <row r="11" spans="1:17" s="3" customFormat="1" ht="124.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="65" t="s">
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="65" t="s">
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="123" t="s">
         <v>55</v>
       </c>
@@ -7612,21 +7654,21 @@
       <c r="Q11" s="125"/>
     </row>
     <row r="12" spans="1:17" s="3" customFormat="1" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="69" t="s">
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="73"/>
       <c r="L12" s="126"/>
       <c r="M12" s="127"/>
       <c r="N12" s="127"/>
@@ -7635,34 +7677,34 @@
       <c r="Q12" s="128"/>
     </row>
     <row r="13" spans="1:17" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="60"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="63"/>
     </row>
     <row r="14" spans="1:17" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="64"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="106" t="s">
         <v>98</v>
       </c>
@@ -7698,184 +7740,184 @@
       <c r="A15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="81"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="84"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="85"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="88"/>
       <c r="K15" s="12"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
-      <c r="N15" s="86"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="88"/>
+      <c r="N15" s="89"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="91"/>
       <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="1:17" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="81"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="85"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="88"/>
       <c r="K16" s="12"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="86"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="88"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="90"/>
+      <c r="P16" s="91"/>
       <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="84"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="85"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="88"/>
       <c r="K17" s="12"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
-      <c r="N17" s="86"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="88"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="91"/>
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="83"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="81"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="84"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="85"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="88"/>
       <c r="K18" s="12"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
-      <c r="N18" s="86"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="88"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="91"/>
       <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="83"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="81"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="84"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="85"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="88"/>
       <c r="K19" s="12"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
-      <c r="N19" s="86"/>
-      <c r="O19" s="87"/>
-      <c r="P19" s="88"/>
+      <c r="N19" s="89"/>
+      <c r="O19" s="90"/>
+      <c r="P19" s="91"/>
       <c r="Q19" s="10"/>
     </row>
     <row r="20" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="83"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="81"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="84"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="84"/>
-      <c r="J20" s="85"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="88"/>
       <c r="K20" s="12"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
-      <c r="N20" s="86"/>
-      <c r="O20" s="87"/>
-      <c r="P20" s="88"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="90"/>
+      <c r="P20" s="91"/>
       <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="81"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="85"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="88"/>
       <c r="K21" s="12"/>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
-      <c r="N21" s="86"/>
-      <c r="O21" s="87"/>
-      <c r="P21" s="88"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="90"/>
+      <c r="P21" s="91"/>
       <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="83"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="81"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="84"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="85"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="88"/>
       <c r="K22" s="12"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
-      <c r="N22" s="86"/>
-      <c r="O22" s="87"/>
-      <c r="P22" s="88"/>
+      <c r="N22" s="89"/>
+      <c r="O22" s="90"/>
+      <c r="P22" s="91"/>
       <c r="Q22" s="10"/>
     </row>
     <row r="23" spans="1:20" s="6" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>